<commit_message>
last uapdate at all
</commit_message>
<xml_diff>
--- a/Etiquette/EtiquettePrintedFile075.xlsx
+++ b/Etiquette/EtiquettePrintedFile075.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etudes20\PycharmProjects\Trial\Etiquette\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E24292-91FB-481D-B074-BECE4B99BB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EtiquettePrintedFile" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -901,8 +907,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -955,11 +961,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1001,7 +1015,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1033,9 +1047,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1067,6 +1099,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1242,14 +1292,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G376"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1272,7 +1333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1293,7 +1354,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1314,7 +1375,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1335,7 +1396,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1356,7 +1417,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1377,7 +1438,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1398,7 +1459,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1419,7 +1480,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -1440,7 +1501,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -1461,7 +1522,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -1482,7 +1543,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1503,7 +1564,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -1524,7 +1585,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -1545,7 +1606,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1566,7 +1627,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1587,7 +1648,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1608,7 +1669,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -1629,7 +1690,7 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -1650,7 +1711,7 @@
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -1671,7 +1732,7 @@
       </c>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -1692,7 +1753,7 @@
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -1713,7 +1774,7 @@
       </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
@@ -1734,7 +1795,7 @@
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -1755,7 +1816,7 @@
       </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -1776,7 +1837,7 @@
       </c>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -1797,7 +1858,7 @@
       </c>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -1818,7 +1879,7 @@
       </c>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
@@ -1839,7 +1900,7 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
@@ -1860,7 +1921,7 @@
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>47</v>
       </c>
@@ -1881,7 +1942,7 @@
       </c>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
@@ -1902,7 +1963,7 @@
       </c>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>47</v>
       </c>
@@ -1923,7 +1984,7 @@
       </c>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>51</v>
       </c>
@@ -1944,7 +2005,7 @@
       </c>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>51</v>
       </c>
@@ -1965,7 +2026,7 @@
       </c>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>53</v>
       </c>
@@ -1986,7 +2047,7 @@
       </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>54</v>
       </c>
@@ -2007,7 +2068,7 @@
       </c>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
@@ -2028,7 +2089,7 @@
       </c>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>56</v>
       </c>
@@ -2049,7 +2110,7 @@
       </c>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>56</v>
       </c>
@@ -2070,7 +2131,7 @@
       </c>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>56</v>
       </c>
@@ -2091,7 +2152,7 @@
       </c>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>56</v>
       </c>
@@ -2112,7 +2173,7 @@
       </c>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -2133,7 +2194,7 @@
       </c>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>63</v>
       </c>
@@ -2154,7 +2215,7 @@
       </c>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -2175,7 +2236,7 @@
       </c>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>68</v>
       </c>
@@ -2196,7 +2257,7 @@
       </c>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>68</v>
       </c>
@@ -2217,7 +2278,7 @@
       </c>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
@@ -2238,7 +2299,7 @@
       </c>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>68</v>
       </c>
@@ -2259,7 +2320,7 @@
       </c>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>65</v>
       </c>
@@ -2280,7 +2341,7 @@
       </c>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>71</v>
       </c>
@@ -2301,7 +2362,7 @@
       </c>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>74</v>
       </c>
@@ -2322,7 +2383,7 @@
       </c>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>75</v>
       </c>
@@ -2343,7 +2404,7 @@
       </c>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>76</v>
       </c>
@@ -2364,7 +2425,7 @@
       </c>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>77</v>
       </c>
@@ -2385,7 +2446,7 @@
       </c>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>78</v>
       </c>
@@ -2406,7 +2467,7 @@
       </c>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>79</v>
       </c>
@@ -2427,7 +2488,7 @@
       </c>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>80</v>
       </c>
@@ -2448,7 +2509,7 @@
       </c>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>81</v>
       </c>
@@ -2469,7 +2530,7 @@
       </c>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>82</v>
       </c>
@@ -2490,7 +2551,7 @@
       </c>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>83</v>
       </c>
@@ -2511,7 +2572,7 @@
       </c>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>84</v>
       </c>
@@ -2532,7 +2593,7 @@
       </c>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>85</v>
       </c>
@@ -2553,7 +2614,7 @@
       </c>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>86</v>
       </c>
@@ -2574,7 +2635,7 @@
       </c>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>87</v>
       </c>
@@ -2595,7 +2656,7 @@
       </c>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>88</v>
       </c>
@@ -2616,7 +2677,7 @@
       </c>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>89</v>
       </c>
@@ -2637,7 +2698,7 @@
       </c>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>90</v>
       </c>
@@ -2658,7 +2719,7 @@
       </c>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>91</v>
       </c>
@@ -2679,7 +2740,7 @@
       </c>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>92</v>
       </c>
@@ -2700,7 +2761,7 @@
       </c>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>93</v>
       </c>
@@ -2721,7 +2782,7 @@
       </c>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>94</v>
       </c>
@@ -2742,7 +2803,7 @@
       </c>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>95</v>
       </c>
@@ -2763,7 +2824,7 @@
       </c>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>97</v>
       </c>
@@ -2784,7 +2845,7 @@
       </c>
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>98</v>
       </c>
@@ -2805,7 +2866,7 @@
       </c>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>99</v>
       </c>
@@ -2826,7 +2887,7 @@
       </c>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>95</v>
       </c>
@@ -2847,7 +2908,7 @@
       </c>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>98</v>
       </c>
@@ -2868,7 +2929,7 @@
       </c>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>98</v>
       </c>
@@ -2889,7 +2950,7 @@
       </c>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>99</v>
       </c>
@@ -2910,7 +2971,7 @@
       </c>
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>98</v>
       </c>
@@ -2931,7 +2992,7 @@
       </c>
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>103</v>
       </c>
@@ -2952,7 +3013,7 @@
       </c>
       <c r="G81" s="1"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>103</v>
       </c>
@@ -2973,7 +3034,7 @@
       </c>
       <c r="G82" s="1"/>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>105</v>
       </c>
@@ -2994,7 +3055,7 @@
       </c>
       <c r="G83" s="1"/>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>103</v>
       </c>
@@ -3015,7 +3076,7 @@
       </c>
       <c r="G84" s="1"/>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>107</v>
       </c>
@@ -3036,7 +3097,7 @@
       </c>
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>105</v>
       </c>
@@ -3057,7 +3118,7 @@
       </c>
       <c r="G86" s="1"/>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>103</v>
       </c>
@@ -3078,7 +3139,7 @@
       </c>
       <c r="G87" s="1"/>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>109</v>
       </c>
@@ -3099,7 +3160,7 @@
       </c>
       <c r="G88" s="1"/>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>105</v>
       </c>
@@ -3120,7 +3181,7 @@
       </c>
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>110</v>
       </c>
@@ -3141,7 +3202,7 @@
       </c>
       <c r="G90" s="1"/>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>112</v>
       </c>
@@ -3162,7 +3223,7 @@
       </c>
       <c r="G91" s="1"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>110</v>
       </c>
@@ -3183,7 +3244,7 @@
       </c>
       <c r="G92" s="1"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>114</v>
       </c>
@@ -3204,7 +3265,7 @@
       </c>
       <c r="G93" s="1"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>109</v>
       </c>
@@ -3225,7 +3286,7 @@
       </c>
       <c r="G94" s="1"/>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>117</v>
       </c>
@@ -3246,7 +3307,7 @@
       </c>
       <c r="G95" s="1"/>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>109</v>
       </c>
@@ -3267,7 +3328,7 @@
       </c>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>110</v>
       </c>
@@ -3288,7 +3349,7 @@
       </c>
       <c r="G97" s="1"/>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>119</v>
       </c>
@@ -3309,7 +3370,7 @@
       </c>
       <c r="G98" s="1"/>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>121</v>
       </c>
@@ -3330,7 +3391,7 @@
       </c>
       <c r="G99" s="1"/>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>122</v>
       </c>
@@ -3351,7 +3412,7 @@
       </c>
       <c r="G100" s="1"/>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>123</v>
       </c>
@@ -3372,7 +3433,7 @@
       </c>
       <c r="G101" s="1"/>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>121</v>
       </c>
@@ -3393,7 +3454,7 @@
       </c>
       <c r="G102" s="1"/>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>125</v>
       </c>
@@ -3414,7 +3475,7 @@
       </c>
       <c r="G103" s="1"/>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>121</v>
       </c>
@@ -3435,7 +3496,7 @@
       </c>
       <c r="G104" s="1"/>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>127</v>
       </c>
@@ -3456,7 +3517,7 @@
       </c>
       <c r="G105" s="1"/>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>125</v>
       </c>
@@ -3477,7 +3538,7 @@
       </c>
       <c r="G106" s="1"/>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>127</v>
       </c>
@@ -3498,7 +3559,7 @@
       </c>
       <c r="G107" s="1"/>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>129</v>
       </c>
@@ -3519,7 +3580,7 @@
       </c>
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>97</v>
       </c>
@@ -3540,7 +3601,7 @@
       </c>
       <c r="G109" s="1"/>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>130</v>
       </c>
@@ -3561,7 +3622,7 @@
       </c>
       <c r="G110" s="1"/>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>16</v>
       </c>
@@ -3582,7 +3643,7 @@
       </c>
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>16</v>
       </c>
@@ -3603,7 +3664,7 @@
       </c>
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>18</v>
       </c>
@@ -3624,7 +3685,7 @@
       </c>
       <c r="G113" s="1"/>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>18</v>
       </c>
@@ -3645,7 +3706,7 @@
       </c>
       <c r="G114" s="1"/>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>97</v>
       </c>
@@ -3666,7 +3727,7 @@
       </c>
       <c r="G115" s="1"/>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>132</v>
       </c>
@@ -3687,7 +3748,7 @@
       </c>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>97</v>
       </c>
@@ -3708,7 +3769,7 @@
       </c>
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>134</v>
       </c>
@@ -3729,7 +3790,7 @@
       </c>
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>132</v>
       </c>
@@ -3750,7 +3811,7 @@
       </c>
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>132</v>
       </c>
@@ -3771,7 +3832,7 @@
       </c>
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>79</v>
       </c>
@@ -3792,7 +3853,7 @@
       </c>
       <c r="G121" s="1"/>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>134</v>
       </c>
@@ -3813,7 +3874,7 @@
       </c>
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>95</v>
       </c>
@@ -3834,7 +3895,7 @@
       </c>
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>119</v>
       </c>
@@ -3855,7 +3916,7 @@
       </c>
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>98</v>
       </c>
@@ -3876,7 +3937,7 @@
       </c>
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>99</v>
       </c>
@@ -3897,7 +3958,7 @@
       </c>
       <c r="G126" s="1"/>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>119</v>
       </c>
@@ -3918,7 +3979,7 @@
       </c>
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>123</v>
       </c>
@@ -3939,7 +4000,7 @@
       </c>
       <c r="G128" s="1"/>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>122</v>
       </c>
@@ -3960,7 +4021,7 @@
       </c>
       <c r="G129" s="1"/>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>119</v>
       </c>
@@ -3981,7 +4042,7 @@
       </c>
       <c r="G130" s="1"/>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>139</v>
       </c>
@@ -4002,7 +4063,7 @@
       </c>
       <c r="G131" s="1"/>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>119</v>
       </c>
@@ -4023,7 +4084,7 @@
       </c>
       <c r="G132" s="1"/>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>141</v>
       </c>
@@ -4044,7 +4105,7 @@
       </c>
       <c r="G133" s="1"/>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>139</v>
       </c>
@@ -4065,7 +4126,7 @@
       </c>
       <c r="G134" s="1"/>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>122</v>
       </c>
@@ -4086,7 +4147,7 @@
       </c>
       <c r="G135" s="1"/>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>141</v>
       </c>
@@ -4107,7 +4168,7 @@
       </c>
       <c r="G136" s="1"/>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>90</v>
       </c>
@@ -4128,7 +4189,7 @@
       </c>
       <c r="G137" s="1"/>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>141</v>
       </c>
@@ -4149,7 +4210,7 @@
       </c>
       <c r="G138" s="1"/>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>144</v>
       </c>
@@ -4170,7 +4231,7 @@
       </c>
       <c r="G139" s="1"/>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>141</v>
       </c>
@@ -4191,7 +4252,7 @@
       </c>
       <c r="G140" s="1"/>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>146</v>
       </c>
@@ -4212,7 +4273,7 @@
       </c>
       <c r="G141" s="1"/>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>147</v>
       </c>
@@ -4233,7 +4294,7 @@
       </c>
       <c r="G142" s="1"/>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>148</v>
       </c>
@@ -4254,7 +4315,7 @@
       </c>
       <c r="G143" s="1"/>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>146</v>
       </c>
@@ -4275,7 +4336,7 @@
       </c>
       <c r="G144" s="1"/>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>146</v>
       </c>
@@ -4296,7 +4357,7 @@
       </c>
       <c r="G145" s="1"/>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>147</v>
       </c>
@@ -4317,7 +4378,7 @@
       </c>
       <c r="G146" s="1"/>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>144</v>
       </c>
@@ -4338,7 +4399,7 @@
       </c>
       <c r="G147" s="1"/>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>151</v>
       </c>
@@ -4359,7 +4420,7 @@
       </c>
       <c r="G148" s="1"/>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>151</v>
       </c>
@@ -4380,7 +4441,7 @@
       </c>
       <c r="G149" s="1"/>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>91</v>
       </c>
@@ -4401,7 +4462,7 @@
       </c>
       <c r="G150" s="1"/>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>153</v>
       </c>
@@ -4422,7 +4483,7 @@
       </c>
       <c r="G151" s="1"/>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>151</v>
       </c>
@@ -4443,7 +4504,7 @@
       </c>
       <c r="G152" s="1"/>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>21</v>
       </c>
@@ -4464,7 +4525,7 @@
       </c>
       <c r="G153" s="1"/>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>21</v>
       </c>
@@ -4485,7 +4546,7 @@
       </c>
       <c r="G154" s="1"/>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>26</v>
       </c>
@@ -4506,7 +4567,7 @@
       </c>
       <c r="G155" s="1"/>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>26</v>
       </c>
@@ -4527,7 +4588,7 @@
       </c>
       <c r="G156" s="1"/>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>29</v>
       </c>
@@ -4548,7 +4609,7 @@
       </c>
       <c r="G157" s="1"/>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>29</v>
       </c>
@@ -4569,7 +4630,7 @@
       </c>
       <c r="G158" s="1"/>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>31</v>
       </c>
@@ -4590,7 +4651,7 @@
       </c>
       <c r="G159" s="1"/>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>154</v>
       </c>
@@ -4611,7 +4672,7 @@
       </c>
       <c r="G160" s="1"/>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>32</v>
       </c>
@@ -4632,7 +4693,7 @@
       </c>
       <c r="G161" s="1"/>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>156</v>
       </c>
@@ -4653,7 +4714,7 @@
       </c>
       <c r="G162" s="1"/>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>32</v>
       </c>
@@ -4674,7 +4735,7 @@
       </c>
       <c r="G163" s="1"/>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>37</v>
       </c>
@@ -4695,7 +4756,7 @@
       </c>
       <c r="G164" s="1"/>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>37</v>
       </c>
@@ -4716,7 +4777,7 @@
       </c>
       <c r="G165" s="1"/>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>39</v>
       </c>
@@ -4737,7 +4798,7 @@
       </c>
       <c r="G166" s="1"/>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>37</v>
       </c>
@@ -4758,7 +4819,7 @@
       </c>
       <c r="G167" s="1"/>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>41</v>
       </c>
@@ -4779,7 +4840,7 @@
       </c>
       <c r="G168" s="1"/>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>41</v>
       </c>
@@ -4800,7 +4861,7 @@
       </c>
       <c r="G169" s="1"/>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>75</v>
       </c>
@@ -4821,7 +4882,7 @@
       </c>
       <c r="G170" s="1"/>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>74</v>
       </c>
@@ -4842,7 +4903,7 @@
       </c>
       <c r="G171" s="1"/>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>71</v>
       </c>
@@ -4863,7 +4924,7 @@
       </c>
       <c r="G172" s="1"/>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>76</v>
       </c>
@@ -4884,7 +4945,7 @@
       </c>
       <c r="G173" s="1"/>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>41</v>
       </c>
@@ -4905,7 +4966,7 @@
       </c>
       <c r="G174" s="1"/>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>76</v>
       </c>
@@ -4926,7 +4987,7 @@
       </c>
       <c r="G175" s="1"/>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>71</v>
       </c>
@@ -4947,7 +5008,7 @@
       </c>
       <c r="G176" s="1"/>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>154</v>
       </c>
@@ -4968,7 +5029,7 @@
       </c>
       <c r="G177" s="1"/>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>158</v>
       </c>
@@ -4989,7 +5050,7 @@
       </c>
       <c r="G178" s="1"/>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>154</v>
       </c>
@@ -5010,7 +5071,7 @@
       </c>
       <c r="G179" s="1"/>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>160</v>
       </c>
@@ -5031,7 +5092,7 @@
       </c>
       <c r="G180" s="1"/>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>158</v>
       </c>
@@ -5052,7 +5113,7 @@
       </c>
       <c r="G181" s="1"/>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>160</v>
       </c>
@@ -5073,7 +5134,7 @@
       </c>
       <c r="G182" s="1"/>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>162</v>
       </c>
@@ -5094,7 +5155,7 @@
       </c>
       <c r="G183" s="1"/>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>163</v>
       </c>
@@ -5115,7 +5176,7 @@
       </c>
       <c r="G184" s="1"/>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>164</v>
       </c>
@@ -5136,7 +5197,7 @@
       </c>
       <c r="G185" s="1"/>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>162</v>
       </c>
@@ -5157,7 +5218,7 @@
       </c>
       <c r="G186" s="1"/>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>165</v>
       </c>
@@ -5178,7 +5239,7 @@
       </c>
       <c r="G187" s="1"/>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>162</v>
       </c>
@@ -5199,7 +5260,7 @@
       </c>
       <c r="G188" s="1"/>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>163</v>
       </c>
@@ -5220,7 +5281,7 @@
       </c>
       <c r="G189" s="1"/>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>163</v>
       </c>
@@ -5241,7 +5302,7 @@
       </c>
       <c r="G190" s="1"/>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>168</v>
       </c>
@@ -5262,7 +5323,7 @@
       </c>
       <c r="G191" s="1"/>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>168</v>
       </c>
@@ -5283,7 +5344,7 @@
       </c>
       <c r="G192" s="1"/>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>170</v>
       </c>
@@ -5304,7 +5365,7 @@
       </c>
       <c r="G193" s="1"/>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>170</v>
       </c>
@@ -5325,7 +5386,7 @@
       </c>
       <c r="G194" s="1"/>
     </row>
-    <row r="195" spans="1:7">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>172</v>
       </c>
@@ -5346,7 +5407,7 @@
       </c>
       <c r="G195" s="1"/>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>172</v>
       </c>
@@ -5367,7 +5428,7 @@
       </c>
       <c r="G196" s="1"/>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>174</v>
       </c>
@@ -5388,7 +5449,7 @@
       </c>
       <c r="G197" s="1"/>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>174</v>
       </c>
@@ -5409,7 +5470,7 @@
       </c>
       <c r="G198" s="1"/>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>176</v>
       </c>
@@ -5430,7 +5491,7 @@
       </c>
       <c r="G199" s="1"/>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>177</v>
       </c>
@@ -5451,7 +5512,7 @@
       </c>
       <c r="G200" s="1"/>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>176</v>
       </c>
@@ -5472,7 +5533,7 @@
       </c>
       <c r="G201" s="1"/>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>179</v>
       </c>
@@ -5493,7 +5554,7 @@
       </c>
       <c r="G202" s="1"/>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>176</v>
       </c>
@@ -5514,7 +5575,7 @@
       </c>
       <c r="G203" s="1"/>
     </row>
-    <row r="204" spans="1:7">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>181</v>
       </c>
@@ -5535,7 +5596,7 @@
       </c>
       <c r="G204" s="1"/>
     </row>
-    <row r="205" spans="1:7">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>182</v>
       </c>
@@ -5556,7 +5617,7 @@
       </c>
       <c r="G205" s="1"/>
     </row>
-    <row r="206" spans="1:7">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>181</v>
       </c>
@@ -5577,7 +5638,7 @@
       </c>
       <c r="G206" s="1"/>
     </row>
-    <row r="207" spans="1:7">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>184</v>
       </c>
@@ -5598,7 +5659,7 @@
       </c>
       <c r="G207" s="1"/>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>160</v>
       </c>
@@ -5619,7 +5680,7 @@
       </c>
       <c r="G208" s="1"/>
     </row>
-    <row r="209" spans="1:7">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>185</v>
       </c>
@@ -5640,7 +5701,7 @@
       </c>
       <c r="G209" s="1"/>
     </row>
-    <row r="210" spans="1:7">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>186</v>
       </c>
@@ -5661,7 +5722,7 @@
       </c>
       <c r="G210" s="1"/>
     </row>
-    <row r="211" spans="1:7">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>185</v>
       </c>
@@ -5682,7 +5743,7 @@
       </c>
       <c r="G211" s="1"/>
     </row>
-    <row r="212" spans="1:7">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>83</v>
       </c>
@@ -5703,7 +5764,7 @@
       </c>
       <c r="G212" s="1"/>
     </row>
-    <row r="213" spans="1:7">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>83</v>
       </c>
@@ -5724,7 +5785,7 @@
       </c>
       <c r="G213" s="1"/>
     </row>
-    <row r="214" spans="1:7">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>47</v>
       </c>
@@ -5745,7 +5806,7 @@
       </c>
       <c r="G214" s="1"/>
     </row>
-    <row r="215" spans="1:7">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>47</v>
       </c>
@@ -5766,7 +5827,7 @@
       </c>
       <c r="G215" s="1"/>
     </row>
-    <row r="216" spans="1:7">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>53</v>
       </c>
@@ -5787,7 +5848,7 @@
       </c>
       <c r="G216" s="1"/>
     </row>
-    <row r="217" spans="1:7">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>54</v>
       </c>
@@ -5808,7 +5869,7 @@
       </c>
       <c r="G217" s="1"/>
     </row>
-    <row r="218" spans="1:7">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>53</v>
       </c>
@@ -5829,7 +5890,7 @@
       </c>
       <c r="G218" s="1"/>
     </row>
-    <row r="219" spans="1:7">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>82</v>
       </c>
@@ -5850,7 +5911,7 @@
       </c>
       <c r="G219" s="1"/>
     </row>
-    <row r="220" spans="1:7">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>82</v>
       </c>
@@ -5871,7 +5932,7 @@
       </c>
       <c r="G220" s="1"/>
     </row>
-    <row r="221" spans="1:7">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>80</v>
       </c>
@@ -5892,7 +5953,7 @@
       </c>
       <c r="G221" s="1"/>
     </row>
-    <row r="222" spans="1:7">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>81</v>
       </c>
@@ -5913,7 +5974,7 @@
       </c>
       <c r="G222" s="1"/>
     </row>
-    <row r="223" spans="1:7">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>160</v>
       </c>
@@ -5934,7 +5995,7 @@
       </c>
       <c r="G223" s="1"/>
     </row>
-    <row r="224" spans="1:7">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>190</v>
       </c>
@@ -5955,7 +6016,7 @@
       </c>
       <c r="G224" s="1"/>
     </row>
-    <row r="225" spans="1:7">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>164</v>
       </c>
@@ -5976,7 +6037,7 @@
       </c>
       <c r="G225" s="1"/>
     </row>
-    <row r="226" spans="1:7">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>160</v>
       </c>
@@ -5997,7 +6058,7 @@
       </c>
       <c r="G226" s="1"/>
     </row>
-    <row r="227" spans="1:7">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>84</v>
       </c>
@@ -6018,7 +6079,7 @@
       </c>
       <c r="G227" s="1"/>
     </row>
-    <row r="228" spans="1:7">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>165</v>
       </c>
@@ -6039,7 +6100,7 @@
       </c>
       <c r="G228" s="1"/>
     </row>
-    <row r="229" spans="1:7">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>164</v>
       </c>
@@ -6060,7 +6121,7 @@
       </c>
       <c r="G229" s="1"/>
     </row>
-    <row r="230" spans="1:7">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>165</v>
       </c>
@@ -6081,7 +6142,7 @@
       </c>
       <c r="G230" s="1"/>
     </row>
-    <row r="231" spans="1:7">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>84</v>
       </c>
@@ -6102,7 +6163,7 @@
       </c>
       <c r="G231" s="1"/>
     </row>
-    <row r="232" spans="1:7">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>56</v>
       </c>
@@ -6123,7 +6184,7 @@
       </c>
       <c r="G232" s="1"/>
     </row>
-    <row r="233" spans="1:7">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>56</v>
       </c>
@@ -6144,7 +6205,7 @@
       </c>
       <c r="G233" s="1"/>
     </row>
-    <row r="234" spans="1:7">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>78</v>
       </c>
@@ -6165,7 +6226,7 @@
       </c>
       <c r="G234" s="1"/>
     </row>
-    <row r="235" spans="1:7">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>78</v>
       </c>
@@ -6186,7 +6247,7 @@
       </c>
       <c r="G235" s="1"/>
     </row>
-    <row r="236" spans="1:7">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>193</v>
       </c>
@@ -6207,7 +6268,7 @@
       </c>
       <c r="G236" s="1"/>
     </row>
-    <row r="237" spans="1:7">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>160</v>
       </c>
@@ -6228,7 +6289,7 @@
       </c>
       <c r="G237" s="1"/>
     </row>
-    <row r="238" spans="1:7">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>194</v>
       </c>
@@ -6249,7 +6310,7 @@
       </c>
       <c r="G238" s="1"/>
     </row>
-    <row r="239" spans="1:7">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>164</v>
       </c>
@@ -6270,7 +6331,7 @@
       </c>
       <c r="G239" s="1"/>
     </row>
-    <row r="240" spans="1:7">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>165</v>
       </c>
@@ -6291,7 +6352,7 @@
       </c>
       <c r="G240" s="1"/>
     </row>
-    <row r="241" spans="1:7">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>84</v>
       </c>
@@ -6312,7 +6373,7 @@
       </c>
       <c r="G241" s="1"/>
     </row>
-    <row r="242" spans="1:7">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>56</v>
       </c>
@@ -6333,7 +6394,7 @@
       </c>
       <c r="G242" s="1"/>
     </row>
-    <row r="243" spans="1:7">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>78</v>
       </c>
@@ -6354,7 +6415,7 @@
       </c>
       <c r="G243" s="1"/>
     </row>
-    <row r="244" spans="1:7">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>193</v>
       </c>
@@ -6375,7 +6436,7 @@
       </c>
       <c r="G244" s="1"/>
     </row>
-    <row r="245" spans="1:7">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>194</v>
       </c>
@@ -6396,7 +6457,7 @@
       </c>
       <c r="G245" s="1"/>
     </row>
-    <row r="246" spans="1:7">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>85</v>
       </c>
@@ -6417,7 +6478,7 @@
       </c>
       <c r="G246" s="1"/>
     </row>
-    <row r="247" spans="1:7">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>196</v>
       </c>
@@ -6438,7 +6499,7 @@
       </c>
       <c r="G247" s="1"/>
     </row>
-    <row r="248" spans="1:7">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>160</v>
       </c>
@@ -6459,7 +6520,7 @@
       </c>
       <c r="G248" s="1"/>
     </row>
-    <row r="249" spans="1:7">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>197</v>
       </c>
@@ -6480,7 +6541,7 @@
       </c>
       <c r="G249" s="1"/>
     </row>
-    <row r="250" spans="1:7">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>77</v>
       </c>
@@ -6501,7 +6562,7 @@
       </c>
       <c r="G250" s="1"/>
     </row>
-    <row r="251" spans="1:7">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>164</v>
       </c>
@@ -6522,7 +6583,7 @@
       </c>
       <c r="G251" s="1"/>
     </row>
-    <row r="252" spans="1:7">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>165</v>
       </c>
@@ -6543,7 +6604,7 @@
       </c>
       <c r="G252" s="1"/>
     </row>
-    <row r="253" spans="1:7">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>84</v>
       </c>
@@ -6564,7 +6625,7 @@
       </c>
       <c r="G253" s="1"/>
     </row>
-    <row r="254" spans="1:7">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>56</v>
       </c>
@@ -6585,7 +6646,7 @@
       </c>
       <c r="G254" s="1"/>
     </row>
-    <row r="255" spans="1:7">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>78</v>
       </c>
@@ -6606,7 +6667,7 @@
       </c>
       <c r="G255" s="1"/>
     </row>
-    <row r="256" spans="1:7">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>193</v>
       </c>
@@ -6627,7 +6688,7 @@
       </c>
       <c r="G256" s="1"/>
     </row>
-    <row r="257" spans="1:7">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>197</v>
       </c>
@@ -6648,7 +6709,7 @@
       </c>
       <c r="G257" s="1"/>
     </row>
-    <row r="258" spans="1:7">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>77</v>
       </c>
@@ -6669,7 +6730,7 @@
       </c>
       <c r="G258" s="1"/>
     </row>
-    <row r="259" spans="1:7">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>197</v>
       </c>
@@ -6690,7 +6751,7 @@
       </c>
       <c r="G259" s="1"/>
     </row>
-    <row r="260" spans="1:7">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>200</v>
       </c>
@@ -6711,7 +6772,7 @@
       </c>
       <c r="G260" s="1"/>
     </row>
-    <row r="261" spans="1:7">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>197</v>
       </c>
@@ -6732,7 +6793,7 @@
       </c>
       <c r="G261" s="1"/>
     </row>
-    <row r="262" spans="1:7">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>202</v>
       </c>
@@ -6753,7 +6814,7 @@
       </c>
       <c r="G262" s="1"/>
     </row>
-    <row r="263" spans="1:7">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>203</v>
       </c>
@@ -6774,7 +6835,7 @@
       </c>
       <c r="G263" s="1"/>
     </row>
-    <row r="264" spans="1:7">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>41</v>
       </c>
@@ -6795,7 +6856,7 @@
       </c>
       <c r="G264" s="1"/>
     </row>
-    <row r="265" spans="1:7">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>63</v>
       </c>
@@ -6816,7 +6877,7 @@
       </c>
       <c r="G265" s="1"/>
     </row>
-    <row r="266" spans="1:7">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>204</v>
       </c>
@@ -6837,7 +6898,7 @@
       </c>
       <c r="G266" s="1"/>
     </row>
-    <row r="267" spans="1:7">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>71</v>
       </c>
@@ -6858,7 +6919,7 @@
       </c>
       <c r="G267" s="1"/>
     </row>
-    <row r="268" spans="1:7">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>76</v>
       </c>
@@ -6879,7 +6940,7 @@
       </c>
       <c r="G268" s="1"/>
     </row>
-    <row r="269" spans="1:7">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>79</v>
       </c>
@@ -6900,7 +6961,7 @@
       </c>
       <c r="G269" s="1"/>
     </row>
-    <row r="270" spans="1:7">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>86</v>
       </c>
@@ -6921,7 +6982,7 @@
       </c>
       <c r="G270" s="1"/>
     </row>
-    <row r="271" spans="1:7">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>87</v>
       </c>
@@ -6942,7 +7003,7 @@
       </c>
       <c r="G271" s="1"/>
     </row>
-    <row r="272" spans="1:7">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>89</v>
       </c>
@@ -6963,7 +7024,7 @@
       </c>
       <c r="G272" s="1"/>
     </row>
-    <row r="273" spans="1:7">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>87</v>
       </c>
@@ -6984,7 +7045,7 @@
       </c>
       <c r="G273" s="1"/>
     </row>
-    <row r="274" spans="1:7">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>88</v>
       </c>
@@ -7005,7 +7066,7 @@
       </c>
       <c r="G274" s="1"/>
     </row>
-    <row r="275" spans="1:7">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>86</v>
       </c>
@@ -7026,7 +7087,7 @@
       </c>
       <c r="G275" s="1"/>
     </row>
-    <row r="276" spans="1:7">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>87</v>
       </c>
@@ -7047,7 +7108,7 @@
       </c>
       <c r="G276" s="1"/>
     </row>
-    <row r="277" spans="1:7">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>119</v>
       </c>
@@ -7068,7 +7129,7 @@
       </c>
       <c r="G277" s="1"/>
     </row>
-    <row r="278" spans="1:7">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>210</v>
       </c>
@@ -7089,7 +7150,7 @@
       </c>
       <c r="G278" s="1"/>
     </row>
-    <row r="279" spans="1:7">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>122</v>
       </c>
@@ -7110,7 +7171,7 @@
       </c>
       <c r="G279" s="1"/>
     </row>
-    <row r="280" spans="1:7">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>123</v>
       </c>
@@ -7131,7 +7192,7 @@
       </c>
       <c r="G280" s="1"/>
     </row>
-    <row r="281" spans="1:7">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>95</v>
       </c>
@@ -7152,7 +7213,7 @@
       </c>
       <c r="G281" s="1"/>
     </row>
-    <row r="282" spans="1:7">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>154</v>
       </c>
@@ -7173,7 +7234,7 @@
       </c>
       <c r="G282" s="1"/>
     </row>
-    <row r="283" spans="1:7">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>98</v>
       </c>
@@ -7194,7 +7255,7 @@
       </c>
       <c r="G283" s="1"/>
     </row>
-    <row r="284" spans="1:7">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>99</v>
       </c>
@@ -7215,7 +7276,7 @@
       </c>
       <c r="G284" s="1"/>
     </row>
-    <row r="285" spans="1:7">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>97</v>
       </c>
@@ -7236,7 +7297,7 @@
       </c>
       <c r="G285" s="1"/>
     </row>
-    <row r="286" spans="1:7">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>65</v>
       </c>
@@ -7257,7 +7318,7 @@
       </c>
       <c r="G286" s="1"/>
     </row>
-    <row r="287" spans="1:7">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>212</v>
       </c>
@@ -7278,7 +7339,7 @@
       </c>
       <c r="G287" s="1"/>
     </row>
-    <row r="288" spans="1:7">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>213</v>
       </c>
@@ -7299,7 +7360,7 @@
       </c>
       <c r="G288" s="1"/>
     </row>
-    <row r="289" spans="1:7">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>214</v>
       </c>
@@ -7320,7 +7381,7 @@
       </c>
       <c r="G289" s="1"/>
     </row>
-    <row r="290" spans="1:7">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>97</v>
       </c>
@@ -7341,7 +7402,7 @@
       </c>
       <c r="G290" s="1"/>
     </row>
-    <row r="291" spans="1:7">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>215</v>
       </c>
@@ -7362,7 +7423,7 @@
       </c>
       <c r="G291" s="1"/>
     </row>
-    <row r="292" spans="1:7">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>214</v>
       </c>
@@ -7383,7 +7444,7 @@
       </c>
       <c r="G292" s="1"/>
     </row>
-    <row r="293" spans="1:7">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>213</v>
       </c>
@@ -7404,7 +7465,7 @@
       </c>
       <c r="G293" s="1"/>
     </row>
-    <row r="294" spans="1:7">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>212</v>
       </c>
@@ -7425,7 +7486,7 @@
       </c>
       <c r="G294" s="1"/>
     </row>
-    <row r="295" spans="1:7">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>65</v>
       </c>
@@ -7446,7 +7507,7 @@
       </c>
       <c r="G295" s="1"/>
     </row>
-    <row r="296" spans="1:7">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>97</v>
       </c>
@@ -7467,7 +7528,7 @@
       </c>
       <c r="G296" s="1"/>
     </row>
-    <row r="297" spans="1:7">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>95</v>
       </c>
@@ -7488,7 +7549,7 @@
       </c>
       <c r="G297" s="1"/>
     </row>
-    <row r="298" spans="1:7">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>216</v>
       </c>
@@ -7509,7 +7570,7 @@
       </c>
       <c r="G298" s="1"/>
     </row>
-    <row r="299" spans="1:7">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>214</v>
       </c>
@@ -7530,7 +7591,7 @@
       </c>
       <c r="G299" s="1"/>
     </row>
-    <row r="300" spans="1:7">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>213</v>
       </c>
@@ -7551,7 +7612,7 @@
       </c>
       <c r="G300" s="1"/>
     </row>
-    <row r="301" spans="1:7">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>212</v>
       </c>
@@ -7572,7 +7633,7 @@
       </c>
       <c r="G301" s="1"/>
     </row>
-    <row r="302" spans="1:7">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>65</v>
       </c>
@@ -7593,7 +7654,7 @@
       </c>
       <c r="G302" s="1"/>
     </row>
-    <row r="303" spans="1:7">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>190</v>
       </c>
@@ -7614,7 +7675,7 @@
       </c>
       <c r="G303" s="1"/>
     </row>
-    <row r="304" spans="1:7">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>218</v>
       </c>
@@ -7635,7 +7696,7 @@
       </c>
       <c r="G304" s="1"/>
     </row>
-    <row r="305" spans="1:7">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>200</v>
       </c>
@@ -7656,7 +7717,7 @@
       </c>
       <c r="G305" s="1"/>
     </row>
-    <row r="306" spans="1:7">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>93</v>
       </c>
@@ -7677,7 +7738,7 @@
       </c>
       <c r="G306" s="1"/>
     </row>
-    <row r="307" spans="1:7">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>132</v>
       </c>
@@ -7698,7 +7759,7 @@
       </c>
       <c r="G307" s="1"/>
     </row>
-    <row r="308" spans="1:7">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>132</v>
       </c>
@@ -7719,7 +7780,7 @@
       </c>
       <c r="G308" s="1"/>
     </row>
-    <row r="309" spans="1:7">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>119</v>
       </c>
@@ -7740,7 +7801,7 @@
       </c>
       <c r="G309" s="1"/>
     </row>
-    <row r="310" spans="1:7">
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>119</v>
       </c>
@@ -7761,7 +7822,7 @@
       </c>
       <c r="G310" s="1"/>
     </row>
-    <row r="311" spans="1:7">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>141</v>
       </c>
@@ -7782,7 +7843,7 @@
       </c>
       <c r="G311" s="1"/>
     </row>
-    <row r="312" spans="1:7">
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>141</v>
       </c>
@@ -7803,7 +7864,7 @@
       </c>
       <c r="G312" s="1"/>
     </row>
-    <row r="313" spans="1:7">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>154</v>
       </c>
@@ -7824,7 +7885,7 @@
       </c>
       <c r="G313" s="1"/>
     </row>
-    <row r="314" spans="1:7">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>154</v>
       </c>
@@ -7845,7 +7906,7 @@
       </c>
       <c r="G314" s="1"/>
     </row>
-    <row r="315" spans="1:7">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>160</v>
       </c>
@@ -7866,7 +7927,7 @@
       </c>
       <c r="G315" s="1"/>
     </row>
-    <row r="316" spans="1:7">
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>160</v>
       </c>
@@ -7887,7 +7948,7 @@
       </c>
       <c r="G316" s="1"/>
     </row>
-    <row r="317" spans="1:7">
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>112</v>
       </c>
@@ -7908,7 +7969,7 @@
       </c>
       <c r="G317" s="1"/>
     </row>
-    <row r="318" spans="1:7">
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>110</v>
       </c>
@@ -7929,7 +7990,7 @@
       </c>
       <c r="G318" s="1"/>
     </row>
-    <row r="319" spans="1:7">
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>117</v>
       </c>
@@ -7950,7 +8011,7 @@
       </c>
       <c r="G319" s="1"/>
     </row>
-    <row r="320" spans="1:7">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>105</v>
       </c>
@@ -7971,7 +8032,7 @@
       </c>
       <c r="G320" s="1"/>
     </row>
-    <row r="321" spans="1:7">
+    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>107</v>
       </c>
@@ -7992,7 +8053,7 @@
       </c>
       <c r="G321" s="1"/>
     </row>
-    <row r="322" spans="1:7">
+    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>109</v>
       </c>
@@ -8013,7 +8074,7 @@
       </c>
       <c r="G322" s="1"/>
     </row>
-    <row r="323" spans="1:7">
+    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>99</v>
       </c>
@@ -8034,7 +8095,7 @@
       </c>
       <c r="G323" s="1"/>
     </row>
-    <row r="324" spans="1:7">
+    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>103</v>
       </c>
@@ -8055,7 +8116,7 @@
       </c>
       <c r="G324" s="1"/>
     </row>
-    <row r="325" spans="1:7">
+    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>95</v>
       </c>
@@ -8076,7 +8137,7 @@
       </c>
       <c r="G325" s="1"/>
     </row>
-    <row r="326" spans="1:7">
+    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>197</v>
       </c>
@@ -8097,7 +8158,7 @@
       </c>
       <c r="G326" s="1"/>
     </row>
-    <row r="327" spans="1:7">
+    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>237</v>
       </c>
@@ -8118,7 +8179,7 @@
       </c>
       <c r="G327" s="1"/>
     </row>
-    <row r="328" spans="1:7">
+    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>141</v>
       </c>
@@ -8139,7 +8200,7 @@
       </c>
       <c r="G328" s="1"/>
     </row>
-    <row r="329" spans="1:7">
+    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>151</v>
       </c>
@@ -8160,7 +8221,7 @@
       </c>
       <c r="G329" s="1"/>
     </row>
-    <row r="330" spans="1:7">
+    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>21</v>
       </c>
@@ -8181,7 +8242,7 @@
       </c>
       <c r="G330" s="1"/>
     </row>
-    <row r="331" spans="1:7">
+    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>26</v>
       </c>
@@ -8202,7 +8263,7 @@
       </c>
       <c r="G331" s="1"/>
     </row>
-    <row r="332" spans="1:7">
+    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>31</v>
       </c>
@@ -8223,7 +8284,7 @@
       </c>
       <c r="G332" s="1"/>
     </row>
-    <row r="333" spans="1:7">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>123</v>
       </c>
@@ -8244,7 +8305,7 @@
       </c>
       <c r="G333" s="1"/>
     </row>
-    <row r="334" spans="1:7">
+    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>119</v>
       </c>
@@ -8265,7 +8326,7 @@
       </c>
       <c r="G334" s="1"/>
     </row>
-    <row r="335" spans="1:7">
+    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>121</v>
       </c>
@@ -8286,7 +8347,7 @@
       </c>
       <c r="G335" s="1"/>
     </row>
-    <row r="336" spans="1:7">
+    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>215</v>
       </c>
@@ -8307,7 +8368,7 @@
       </c>
       <c r="G336" s="1"/>
     </row>
-    <row r="337" spans="1:7">
+    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>32</v>
       </c>
@@ -8328,7 +8389,7 @@
       </c>
       <c r="G337" s="1"/>
     </row>
-    <row r="338" spans="1:7">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>37</v>
       </c>
@@ -8349,7 +8410,7 @@
       </c>
       <c r="G338" s="1"/>
     </row>
-    <row r="339" spans="1:7">
+    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>41</v>
       </c>
@@ -8370,7 +8431,7 @@
       </c>
       <c r="G339" s="1"/>
     </row>
-    <row r="340" spans="1:7">
+    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>29</v>
       </c>
@@ -8391,7 +8452,7 @@
       </c>
       <c r="G340" s="1"/>
     </row>
-    <row r="341" spans="1:7">
+    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>63</v>
       </c>
@@ -8412,7 +8473,7 @@
       </c>
       <c r="G341" s="1"/>
     </row>
-    <row r="342" spans="1:7">
+    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>56</v>
       </c>
@@ -8433,7 +8494,7 @@
       </c>
       <c r="G342" s="1"/>
     </row>
-    <row r="343" spans="1:7">
+    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>179</v>
       </c>
@@ -8454,7 +8515,7 @@
       </c>
       <c r="G343" s="1"/>
     </row>
-    <row r="344" spans="1:7">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>172</v>
       </c>
@@ -8475,7 +8536,7 @@
       </c>
       <c r="G344" s="1"/>
     </row>
-    <row r="345" spans="1:7">
+    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>170</v>
       </c>
@@ -8496,7 +8557,7 @@
       </c>
       <c r="G345" s="1"/>
     </row>
-    <row r="346" spans="1:7">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>168</v>
       </c>
@@ -8517,7 +8578,7 @@
       </c>
       <c r="G346" s="1"/>
     </row>
-    <row r="347" spans="1:7">
+    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>162</v>
       </c>
@@ -8538,7 +8599,7 @@
       </c>
       <c r="G347" s="1"/>
     </row>
-    <row r="348" spans="1:7">
+    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>158</v>
       </c>
@@ -8559,7 +8620,7 @@
       </c>
       <c r="G348" s="1"/>
     </row>
-    <row r="349" spans="1:7">
+    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>194</v>
       </c>
@@ -8580,7 +8641,7 @@
       </c>
       <c r="G349" s="1"/>
     </row>
-    <row r="350" spans="1:7">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>160</v>
       </c>
@@ -8601,7 +8662,7 @@
       </c>
       <c r="G350" s="1"/>
     </row>
-    <row r="351" spans="1:7">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>65</v>
       </c>
@@ -8622,7 +8683,7 @@
       </c>
       <c r="G351" s="1"/>
     </row>
-    <row r="352" spans="1:7">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>12</v>
       </c>
@@ -8643,7 +8704,7 @@
       </c>
       <c r="G352" s="1"/>
     </row>
-    <row r="353" spans="1:7">
+    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>132</v>
       </c>
@@ -8664,7 +8725,7 @@
       </c>
       <c r="G353" s="1"/>
     </row>
-    <row r="354" spans="1:7">
+    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>53</v>
       </c>
@@ -8685,7 +8746,7 @@
       </c>
       <c r="G354" s="1"/>
     </row>
-    <row r="355" spans="1:7">
+    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>51</v>
       </c>
@@ -8706,7 +8767,7 @@
       </c>
       <c r="G355" s="1"/>
     </row>
-    <row r="356" spans="1:7">
+    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>176</v>
       </c>
@@ -8727,7 +8788,7 @@
       </c>
       <c r="G356" s="1"/>
     </row>
-    <row r="357" spans="1:7">
+    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>174</v>
       </c>
@@ -8748,7 +8809,7 @@
       </c>
       <c r="G357" s="1"/>
     </row>
-    <row r="358" spans="1:7">
+    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>163</v>
       </c>
@@ -8769,7 +8830,7 @@
       </c>
       <c r="G358" s="1"/>
     </row>
-    <row r="359" spans="1:7">
+    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>147</v>
       </c>
@@ -8790,7 +8851,7 @@
       </c>
       <c r="G359" s="1"/>
     </row>
-    <row r="360" spans="1:7">
+    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>210</v>
       </c>
@@ -8811,7 +8872,7 @@
       </c>
       <c r="G360" s="1"/>
     </row>
-    <row r="361" spans="1:7">
+    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>98</v>
       </c>
@@ -8832,7 +8893,7 @@
       </c>
       <c r="G361" s="1"/>
     </row>
-    <row r="362" spans="1:7">
+    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>144</v>
       </c>
@@ -8853,7 +8914,7 @@
       </c>
       <c r="G362" s="1"/>
     </row>
-    <row r="363" spans="1:7">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>139</v>
       </c>
@@ -8874,7 +8935,7 @@
       </c>
       <c r="G363" s="1"/>
     </row>
-    <row r="364" spans="1:7">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>47</v>
       </c>
@@ -8895,7 +8956,7 @@
       </c>
       <c r="G364" s="1"/>
     </row>
-    <row r="365" spans="1:7">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
         <v>18</v>
       </c>
@@ -8916,7 +8977,7 @@
       </c>
       <c r="G365" s="1"/>
     </row>
-    <row r="366" spans="1:7">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>16</v>
       </c>
@@ -8937,7 +8998,7 @@
       </c>
       <c r="G366" s="1"/>
     </row>
-    <row r="367" spans="1:7">
+    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>154</v>
       </c>
@@ -8958,7 +9019,7 @@
       </c>
       <c r="G367" s="1"/>
     </row>
-    <row r="368" spans="1:7">
+    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>125</v>
       </c>
@@ -8979,7 +9040,7 @@
       </c>
       <c r="G368" s="1"/>
     </row>
-    <row r="369" spans="1:7">
+    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>39</v>
       </c>
@@ -9000,7 +9061,7 @@
       </c>
       <c r="G369" s="1"/>
     </row>
-    <row r="370" spans="1:7">
+    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>97</v>
       </c>
@@ -9021,7 +9082,7 @@
       </c>
       <c r="G370" s="1"/>
     </row>
-    <row r="371" spans="1:7">
+    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>119</v>
       </c>
@@ -9042,7 +9103,7 @@
       </c>
       <c r="G371" s="1"/>
     </row>
-    <row r="372" spans="1:7">
+    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>154</v>
       </c>
@@ -9063,7 +9124,7 @@
       </c>
       <c r="G372" s="1"/>
     </row>
-    <row r="373" spans="1:7">
+    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>160</v>
       </c>
@@ -9084,7 +9145,7 @@
       </c>
       <c r="G373" s="1"/>
     </row>
-    <row r="374" spans="1:7">
+    <row r="374" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>132</v>
       </c>
@@ -9105,7 +9166,7 @@
       </c>
       <c r="G374" s="1"/>
     </row>
-    <row r="375" spans="1:7">
+    <row r="375" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>141</v>
       </c>
@@ -9126,7 +9187,7 @@
       </c>
       <c r="G375" s="1"/>
     </row>
-    <row r="376" spans="1:7">
+    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>95</v>
       </c>

</xml_diff>